<commit_message>
improved UI, added configurable view port size
</commit_message>
<xml_diff>
--- a/src/Mastersign.AutoForm/Template.xlsx
+++ b/src/Mastersign.AutoForm/Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Repository\Projekte\OS\Mastersign.AutoForm\src\Mastersign.AutoForm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E51176BF-4B8E-49C2-B601-D181BEAF35D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B6BB73F-AA73-4531-A0A1-6D6B7FA63DF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24390" yWindow="1050" windowWidth="23040" windowHeight="18765" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38130" yWindow="270" windowWidth="23040" windowHeight="18765" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Script" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="56">
   <si>
     <t>Name</t>
   </si>
@@ -124,9 +124,6 @@
     <t>div.message div.ready</t>
   </si>
   <si>
-    <t>Section</t>
-  </si>
-  <si>
     <t>#mainForm</t>
   </si>
   <si>
@@ -203,6 +200,15 @@
   </si>
   <si>
     <t>Skip</t>
+  </si>
+  <si>
+    <t>Width</t>
+  </si>
+  <si>
+    <t>Height</t>
+  </si>
+  <si>
+    <t>https://github.com/mastersign/Mastersign.AutoForm/releases</t>
   </si>
 </sst>
 </file>
@@ -315,16 +321,27 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -600,10 +617,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F109"/>
+  <dimension ref="A1:F111"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -620,761 +637,762 @@
       <c r="A1" s="7" t="s">
         <v>2</v>
       </c>
+      <c r="F1" s="11" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="2" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>27</v>
-      </c>
+      <c r="A3" s="6"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
+      <c r="A4" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="A6" s="5"/>
+      <c r="B6" s="2"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
+      <c r="A7" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7">
+        <v>1020</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>20</v>
+      <c r="A8" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8">
+        <v>1220</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F9" s="3" t="str">
-        <f>IF($B9&lt;&gt;"",_xlfn.XLOOKUP($B9,ActionTypes,ActionTypeParameter) &amp; ": " &amp; _xlfn.XLOOKUP($B9,ActionTypes,ActionTypeHelp),"")</f>
-        <v/>
-      </c>
+      <c r="A9" s="5"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
-      <c r="B10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="3" t="str">
-        <f>IF($B10&lt;&gt;"",_xlfn.XLOOKUP($B10,ActionTypes,ActionTypeParameter) &amp; ": " &amp; _xlfn.XLOOKUP($B10,ActionTypes,ActionTypeHelp),"")</f>
-        <v>Url, [Timeout]: Navigate to the given URL. Cancel if timeout in milliseconds is reached.</v>
+      <c r="B10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="10">
-        <v>500</v>
-      </c>
-      <c r="E11" s="10"/>
+      <c r="A11" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
       <c r="F11" s="3" t="str">
-        <f>IF($B11&lt;&gt;"",_xlfn.XLOOKUP($B11,ActionTypes,ActionTypeParameter) &amp; ": " &amp; _xlfn.XLOOKUP($B11,ActionTypes,ActionTypeHelp),"")</f>
-        <v>Selector, [Timeout]: Wait for an element to be present and visible/hidden. Cancel if timeout in milliseconds is reached.</v>
+        <f t="shared" ref="F11:F21" si="0">IF($B11&lt;&gt;"",_xlfn.XLOOKUP($B11,ActionTypes,ActionTypeParameter) &amp; ": " &amp; _xlfn.XLOOKUP($B11,ActionTypes,ActionTypeHelp),"")</f>
+        <v/>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" t="s">
-        <v>42</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
+        <v>6</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
       <c r="F12" s="3" t="str">
-        <f>IF($B12&lt;&gt;"",_xlfn.XLOOKUP($B12,ActionTypes,ActionTypeParameter) &amp; ": " &amp; _xlfn.XLOOKUP($B12,ActionTypes,ActionTypeHelp),"")</f>
-        <v>Selector, [Timeout], …Fields: Wait for a form and fill its fields. Cancel if timeout in milliseconds is reached.</v>
+        <f t="shared" si="0"/>
+        <v>Url, [Timeout]: Navigate to the given URL. Cancel if timeout in milliseconds is reached.</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
-      <c r="C13" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="E13" s="10"/>
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="9">
+        <v>500</v>
+      </c>
+      <c r="E13" s="9"/>
       <c r="F13" s="3" t="str">
-        <f>IF($B13&lt;&gt;"",_xlfn.XLOOKUP($B13,ActionTypes,ActionTypeParameter) &amp; ": " &amp; _xlfn.XLOOKUP($B13,ActionTypes,ActionTypeHelp),"")</f>
-        <v/>
+        <f t="shared" si="0"/>
+        <v>Selector, [Timeout]: Wait for an element to be present and visible/hidden. Cancel if timeout in milliseconds is reached.</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
-      <c r="C14" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="E14" s="10"/>
+      <c r="B14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
       <c r="F14" s="3" t="str">
-        <f>IF($B14&lt;&gt;"",_xlfn.XLOOKUP($B14,ActionTypes,ActionTypeParameter) &amp; ": " &amp; _xlfn.XLOOKUP($B14,ActionTypes,ActionTypeHelp),"")</f>
-        <v/>
+        <f t="shared" si="0"/>
+        <v>Selector, [Timeout], …Fields: Wait for a form and fill its fields. Cancel if timeout in milliseconds is reached.</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
-      <c r="C15" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="E15" s="10"/>
+      <c r="C15" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="9"/>
       <c r="F15" s="3" t="str">
-        <f>IF($B15&lt;&gt;"",_xlfn.XLOOKUP($B15,ActionTypes,ActionTypeParameter) &amp; ": " &amp; _xlfn.XLOOKUP($B15,ActionTypes,ActionTypeHelp),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
-      <c r="C16" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="E16" s="10"/>
+      <c r="C16" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" s="9"/>
       <c r="F16" s="3" t="str">
-        <f>IF($B16&lt;&gt;"",_xlfn.XLOOKUP($B16,ActionTypes,ActionTypeParameter) &amp; ": " &amp; _xlfn.XLOOKUP($B16,ActionTypes,ActionTypeHelp),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
-      <c r="C17" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="E17" s="10"/>
+      <c r="C17" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" s="9"/>
       <c r="F17" s="3" t="str">
-        <f>IF($B17&lt;&gt;"",_xlfn.XLOOKUP($B17,ActionTypes,ActionTypeParameter) &amp; ": " &amp; _xlfn.XLOOKUP($B17,ActionTypes,ActionTypeHelp),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
-      <c r="B18" t="s">
-        <v>8</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="D18" s="11"/>
-      <c r="E18" s="10"/>
+      <c r="C18" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" s="9"/>
       <c r="F18" s="3" t="str">
-        <f>IF($B18&lt;&gt;"",_xlfn.XLOOKUP($B18,ActionTypes,ActionTypeParameter) &amp; ": " &amp; _xlfn.XLOOKUP($B18,ActionTypes,ActionTypeHelp),"")</f>
-        <v>Label: Interrupt the script execution and wait for the user to proceed.</v>
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B19" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
+      <c r="A19" s="5"/>
+      <c r="C19" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E19" s="9"/>
       <c r="F19" s="3" t="str">
-        <f>IF($B19&lt;&gt;"",_xlfn.XLOOKUP($B19,ActionTypes,ActionTypeParameter) &amp; ": " &amp; _xlfn.XLOOKUP($B19,ActionTypes,ActionTypeHelp),"")</f>
-        <v>Selector, [Timeout]: Wait for an element and click on it. Cancel if timeout in milliseconds is reached.</v>
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="10"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Label: Interrupt the script execution and wait for the user to proceed.</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" t="s">
         <v>10</v>
       </c>
-      <c r="C20" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="3" t="str">
-        <f t="shared" ref="F20:F72" si="0">IF($B20&lt;&gt;"",_xlfn.XLOOKUP($B20,ActionTypes,ActionTypeParameter) &amp; ": " &amp; _xlfn.XLOOKUP($B20,ActionTypes,ActionTypeHelp),"")</f>
-        <v>Selector, [Timeout]: Wait for an element and click on it. Cancel if timeout in milliseconds is reached.</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
+      <c r="C21" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
       <c r="F21" s="3" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>Selector, [Timeout]: Wait for an element and click on it. Cancel if timeout in milliseconds is reached.</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
+      <c r="B22" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
       <c r="F22" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+        <f t="shared" ref="F22:F74" si="1">IF($B22&lt;&gt;"",_xlfn.XLOOKUP($B22,ActionTypes,ActionTypeParameter) &amp; ": " &amp; _xlfn.XLOOKUP($B22,ActionTypes,ActionTypeHelp),"")</f>
+        <v>Selector, [Timeout]: Wait for an element and click on it. Cancel if timeout in milliseconds is reached.</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
       <c r="F23" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
       <c r="F24" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
       <c r="F25" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
       <c r="F26" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
       <c r="F27" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="10"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
       <c r="F28" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
       <c r="F29" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="10"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
       <c r="F30" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
       <c r="F31" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="10"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
       <c r="F32" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="10"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
       <c r="F33" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="5"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="10"/>
-      <c r="E34" s="10"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
       <c r="F34" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="5"/>
-      <c r="C35" s="10"/>
-      <c r="D35" s="10"/>
-      <c r="E35" s="10"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
       <c r="F35" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="5"/>
-      <c r="C36" s="10"/>
-      <c r="D36" s="10"/>
-      <c r="E36" s="10"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
       <c r="F36" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="5"/>
-      <c r="C37" s="10"/>
-      <c r="D37" s="10"/>
-      <c r="E37" s="10"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
       <c r="F37" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="5"/>
-      <c r="C38" s="10"/>
-      <c r="D38" s="10"/>
-      <c r="E38" s="10"/>
+      <c r="C38" s="9"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
       <c r="F38" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="5"/>
-      <c r="C39" s="10"/>
-      <c r="D39" s="10"/>
-      <c r="E39" s="10"/>
+      <c r="C39" s="9"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="9"/>
       <c r="F39" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="5"/>
-      <c r="C40" s="10"/>
-      <c r="D40" s="10"/>
-      <c r="E40" s="10"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
       <c r="F40" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="5"/>
-      <c r="C41" s="10"/>
-      <c r="D41" s="10"/>
-      <c r="E41" s="10"/>
+      <c r="C41" s="9"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="9"/>
       <c r="F41" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="5"/>
-      <c r="C42" s="10"/>
-      <c r="D42" s="10"/>
-      <c r="E42" s="10"/>
+      <c r="C42" s="9"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="9"/>
       <c r="F42" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="5"/>
-      <c r="C43" s="10"/>
-      <c r="D43" s="10"/>
-      <c r="E43" s="10"/>
+      <c r="C43" s="9"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="9"/>
       <c r="F43" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="5"/>
-      <c r="C44" s="10"/>
-      <c r="D44" s="10"/>
-      <c r="E44" s="10"/>
+      <c r="C44" s="9"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="9"/>
       <c r="F44" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="5"/>
-      <c r="C45" s="10"/>
-      <c r="D45" s="10"/>
-      <c r="E45" s="10"/>
+      <c r="C45" s="9"/>
+      <c r="D45" s="9"/>
+      <c r="E45" s="9"/>
       <c r="F45" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="5"/>
-      <c r="C46" s="10"/>
-      <c r="D46" s="10"/>
-      <c r="E46" s="10"/>
+      <c r="C46" s="9"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="9"/>
       <c r="F46" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="5"/>
-      <c r="C47" s="10"/>
-      <c r="D47" s="10"/>
-      <c r="E47" s="10"/>
+      <c r="C47" s="9"/>
+      <c r="D47" s="9"/>
+      <c r="E47" s="9"/>
       <c r="F47" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="5"/>
-      <c r="C48" s="10"/>
-      <c r="D48" s="10"/>
-      <c r="E48" s="10"/>
+      <c r="C48" s="9"/>
+      <c r="D48" s="9"/>
+      <c r="E48" s="9"/>
       <c r="F48" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="5"/>
-      <c r="C49" s="10"/>
-      <c r="D49" s="10"/>
-      <c r="E49" s="10"/>
+      <c r="C49" s="9"/>
+      <c r="D49" s="9"/>
+      <c r="E49" s="9"/>
       <c r="F49" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="5"/>
-      <c r="C50" s="10"/>
-      <c r="D50" s="10"/>
-      <c r="E50" s="10"/>
+      <c r="C50" s="9"/>
+      <c r="D50" s="9"/>
+      <c r="E50" s="9"/>
       <c r="F50" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="5"/>
-      <c r="C51" s="10"/>
-      <c r="D51" s="10"/>
-      <c r="E51" s="10"/>
+      <c r="C51" s="9"/>
+      <c r="D51" s="9"/>
+      <c r="E51" s="9"/>
       <c r="F51" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="5"/>
-      <c r="C52" s="10"/>
-      <c r="D52" s="10"/>
-      <c r="E52" s="10"/>
+      <c r="C52" s="9"/>
+      <c r="D52" s="9"/>
+      <c r="E52" s="9"/>
       <c r="F52" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="5"/>
-      <c r="C53" s="10"/>
-      <c r="D53" s="10"/>
-      <c r="E53" s="10"/>
+      <c r="C53" s="9"/>
+      <c r="D53" s="9"/>
+      <c r="E53" s="9"/>
       <c r="F53" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="5"/>
-      <c r="C54" s="10"/>
-      <c r="D54" s="10"/>
-      <c r="E54" s="10"/>
+      <c r="C54" s="9"/>
+      <c r="D54" s="9"/>
+      <c r="E54" s="9"/>
       <c r="F54" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="5"/>
-      <c r="C55" s="10"/>
-      <c r="D55" s="10"/>
-      <c r="E55" s="10"/>
+      <c r="C55" s="9"/>
+      <c r="D55" s="9"/>
+      <c r="E55" s="9"/>
       <c r="F55" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="5"/>
-      <c r="C56" s="10"/>
-      <c r="D56" s="10"/>
-      <c r="E56" s="10"/>
+      <c r="C56" s="9"/>
+      <c r="D56" s="9"/>
+      <c r="E56" s="9"/>
       <c r="F56" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="5"/>
-      <c r="C57" s="10"/>
-      <c r="D57" s="10"/>
-      <c r="E57" s="10"/>
+      <c r="C57" s="9"/>
+      <c r="D57" s="9"/>
+      <c r="E57" s="9"/>
       <c r="F57" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="5"/>
-      <c r="C58" s="10"/>
-      <c r="D58" s="10"/>
-      <c r="E58" s="10"/>
+      <c r="C58" s="9"/>
+      <c r="D58" s="9"/>
+      <c r="E58" s="9"/>
       <c r="F58" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="5"/>
-      <c r="C59" s="10"/>
-      <c r="D59" s="10"/>
-      <c r="E59" s="10"/>
+      <c r="C59" s="9"/>
+      <c r="D59" s="9"/>
+      <c r="E59" s="9"/>
       <c r="F59" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="5"/>
-      <c r="C60" s="10"/>
-      <c r="D60" s="10"/>
-      <c r="E60" s="10"/>
+      <c r="C60" s="9"/>
+      <c r="D60" s="9"/>
+      <c r="E60" s="9"/>
       <c r="F60" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="5"/>
-      <c r="C61" s="10"/>
-      <c r="D61" s="10"/>
-      <c r="E61" s="10"/>
+      <c r="C61" s="9"/>
+      <c r="D61" s="9"/>
+      <c r="E61" s="9"/>
       <c r="F61" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="5"/>
-      <c r="C62" s="10"/>
-      <c r="D62" s="10"/>
-      <c r="E62" s="10"/>
+      <c r="C62" s="9"/>
+      <c r="D62" s="9"/>
+      <c r="E62" s="9"/>
       <c r="F62" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="5"/>
-      <c r="C63" s="10"/>
-      <c r="D63" s="10"/>
-      <c r="E63" s="10"/>
+      <c r="C63" s="9"/>
+      <c r="D63" s="9"/>
+      <c r="E63" s="9"/>
       <c r="F63" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="5"/>
-      <c r="C64" s="10"/>
-      <c r="D64" s="10"/>
-      <c r="E64" s="10"/>
+      <c r="C64" s="9"/>
+      <c r="D64" s="9"/>
+      <c r="E64" s="9"/>
       <c r="F64" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="5"/>
-      <c r="C65" s="10"/>
-      <c r="D65" s="10"/>
-      <c r="E65" s="10"/>
+      <c r="C65" s="9"/>
+      <c r="D65" s="9"/>
+      <c r="E65" s="9"/>
       <c r="F65" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="5"/>
-      <c r="C66" s="10"/>
-      <c r="D66" s="10"/>
-      <c r="E66" s="10"/>
+      <c r="C66" s="9"/>
+      <c r="D66" s="9"/>
+      <c r="E66" s="9"/>
       <c r="F66" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="5"/>
-      <c r="C67" s="10"/>
-      <c r="D67" s="10"/>
-      <c r="E67" s="10"/>
+      <c r="C67" s="9"/>
+      <c r="D67" s="9"/>
+      <c r="E67" s="9"/>
       <c r="F67" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="5"/>
-      <c r="C68" s="10"/>
-      <c r="D68" s="10"/>
-      <c r="E68" s="10"/>
+      <c r="C68" s="9"/>
+      <c r="D68" s="9"/>
+      <c r="E68" s="9"/>
       <c r="F68" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="5"/>
-      <c r="C69" s="10"/>
-      <c r="D69" s="10"/>
-      <c r="E69" s="10"/>
+      <c r="C69" s="9"/>
+      <c r="D69" s="9"/>
+      <c r="E69" s="9"/>
       <c r="F69" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="5"/>
-      <c r="C70" s="10"/>
-      <c r="D70" s="10"/>
-      <c r="E70" s="10"/>
+      <c r="C70" s="9"/>
+      <c r="D70" s="9"/>
+      <c r="E70" s="9"/>
       <c r="F70" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="5"/>
-      <c r="C71" s="10"/>
-      <c r="D71" s="10"/>
-      <c r="E71" s="10"/>
+      <c r="C71" s="9"/>
+      <c r="D71" s="9"/>
+      <c r="E71" s="9"/>
       <c r="F71" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="5"/>
-      <c r="C72" s="10"/>
-      <c r="D72" s="10"/>
-      <c r="E72" s="10"/>
+      <c r="C72" s="9"/>
+      <c r="D72" s="9"/>
+      <c r="E72" s="9"/>
       <c r="F72" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="5"/>
-      <c r="C73" s="10"/>
-      <c r="D73" s="10"/>
-      <c r="E73" s="10"/>
+      <c r="C73" s="9"/>
+      <c r="D73" s="9"/>
+      <c r="E73" s="9"/>
       <c r="F73" s="3" t="str">
-        <f t="shared" ref="F73:F109" si="1">IF($B73&lt;&gt;"",_xlfn.XLOOKUP($B73,ActionTypes,ActionTypeParameter) &amp; ": " &amp; _xlfn.XLOOKUP($B73,ActionTypes,ActionTypeHelp),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="5"/>
-      <c r="C74" s="10"/>
-      <c r="D74" s="10"/>
-      <c r="E74" s="10"/>
+      <c r="C74" s="9"/>
+      <c r="D74" s="9"/>
+      <c r="E74" s="9"/>
       <c r="F74" s="3" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -1382,365 +1400,391 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="5"/>
-      <c r="C75" s="10"/>
-      <c r="D75" s="10"/>
-      <c r="E75" s="10"/>
+      <c r="C75" s="9"/>
+      <c r="D75" s="9"/>
+      <c r="E75" s="9"/>
       <c r="F75" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="F75:F111" si="2">IF($B75&lt;&gt;"",_xlfn.XLOOKUP($B75,ActionTypes,ActionTypeParameter) &amp; ": " &amp; _xlfn.XLOOKUP($B75,ActionTypes,ActionTypeHelp),"")</f>
         <v/>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="5"/>
-      <c r="C76" s="10"/>
-      <c r="D76" s="10"/>
-      <c r="E76" s="10"/>
+      <c r="C76" s="9"/>
+      <c r="D76" s="9"/>
+      <c r="E76" s="9"/>
       <c r="F76" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="5"/>
-      <c r="C77" s="10"/>
-      <c r="D77" s="10"/>
-      <c r="E77" s="10"/>
+      <c r="C77" s="9"/>
+      <c r="D77" s="9"/>
+      <c r="E77" s="9"/>
       <c r="F77" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="5"/>
-      <c r="C78" s="10"/>
-      <c r="D78" s="10"/>
-      <c r="E78" s="10"/>
+      <c r="C78" s="9"/>
+      <c r="D78" s="9"/>
+      <c r="E78" s="9"/>
       <c r="F78" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="5"/>
-      <c r="C79" s="10"/>
-      <c r="D79" s="10"/>
-      <c r="E79" s="10"/>
+      <c r="C79" s="9"/>
+      <c r="D79" s="9"/>
+      <c r="E79" s="9"/>
       <c r="F79" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="5"/>
-      <c r="C80" s="10"/>
-      <c r="D80" s="10"/>
-      <c r="E80" s="10"/>
+      <c r="C80" s="9"/>
+      <c r="D80" s="9"/>
+      <c r="E80" s="9"/>
       <c r="F80" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="5"/>
-      <c r="C81" s="10"/>
-      <c r="D81" s="10"/>
-      <c r="E81" s="10"/>
+      <c r="C81" s="9"/>
+      <c r="D81" s="9"/>
+      <c r="E81" s="9"/>
       <c r="F81" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="5"/>
-      <c r="C82" s="10"/>
-      <c r="D82" s="10"/>
-      <c r="E82" s="10"/>
+      <c r="C82" s="9"/>
+      <c r="D82" s="9"/>
+      <c r="E82" s="9"/>
       <c r="F82" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="5"/>
-      <c r="C83" s="10"/>
-      <c r="D83" s="10"/>
-      <c r="E83" s="10"/>
+      <c r="C83" s="9"/>
+      <c r="D83" s="9"/>
+      <c r="E83" s="9"/>
       <c r="F83" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="5"/>
-      <c r="C84" s="10"/>
-      <c r="D84" s="10"/>
-      <c r="E84" s="10"/>
+      <c r="C84" s="9"/>
+      <c r="D84" s="9"/>
+      <c r="E84" s="9"/>
       <c r="F84" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="5"/>
-      <c r="C85" s="10"/>
-      <c r="D85" s="10"/>
-      <c r="E85" s="10"/>
+      <c r="C85" s="9"/>
+      <c r="D85" s="9"/>
+      <c r="E85" s="9"/>
       <c r="F85" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="5"/>
-      <c r="C86" s="10"/>
-      <c r="D86" s="10"/>
-      <c r="E86" s="10"/>
+      <c r="C86" s="9"/>
+      <c r="D86" s="9"/>
+      <c r="E86" s="9"/>
       <c r="F86" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="5"/>
-      <c r="C87" s="10"/>
-      <c r="D87" s="10"/>
-      <c r="E87" s="10"/>
+      <c r="C87" s="9"/>
+      <c r="D87" s="9"/>
+      <c r="E87" s="9"/>
       <c r="F87" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="5"/>
-      <c r="C88" s="10"/>
-      <c r="D88" s="10"/>
-      <c r="E88" s="10"/>
+      <c r="C88" s="9"/>
+      <c r="D88" s="9"/>
+      <c r="E88" s="9"/>
       <c r="F88" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="5"/>
-      <c r="C89" s="10"/>
-      <c r="D89" s="10"/>
-      <c r="E89" s="10"/>
+      <c r="C89" s="9"/>
+      <c r="D89" s="9"/>
+      <c r="E89" s="9"/>
       <c r="F89" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="5"/>
-      <c r="C90" s="10"/>
-      <c r="D90" s="10"/>
-      <c r="E90" s="10"/>
+      <c r="C90" s="9"/>
+      <c r="D90" s="9"/>
+      <c r="E90" s="9"/>
       <c r="F90" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="5"/>
-      <c r="C91" s="10"/>
-      <c r="D91" s="10"/>
-      <c r="E91" s="10"/>
+      <c r="C91" s="9"/>
+      <c r="D91" s="9"/>
+      <c r="E91" s="9"/>
       <c r="F91" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="5"/>
-      <c r="C92" s="10"/>
-      <c r="D92" s="10"/>
-      <c r="E92" s="10"/>
+      <c r="C92" s="9"/>
+      <c r="D92" s="9"/>
+      <c r="E92" s="9"/>
       <c r="F92" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="5"/>
-      <c r="C93" s="10"/>
-      <c r="D93" s="10"/>
-      <c r="E93" s="10"/>
+      <c r="C93" s="9"/>
+      <c r="D93" s="9"/>
+      <c r="E93" s="9"/>
       <c r="F93" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="5"/>
-      <c r="C94" s="10"/>
-      <c r="D94" s="10"/>
-      <c r="E94" s="10"/>
+      <c r="C94" s="9"/>
+      <c r="D94" s="9"/>
+      <c r="E94" s="9"/>
       <c r="F94" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="5"/>
-      <c r="C95" s="10"/>
-      <c r="D95" s="10"/>
-      <c r="E95" s="10"/>
+      <c r="C95" s="9"/>
+      <c r="D95" s="9"/>
+      <c r="E95" s="9"/>
       <c r="F95" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="5"/>
-      <c r="C96" s="10"/>
-      <c r="D96" s="10"/>
-      <c r="E96" s="10"/>
+      <c r="C96" s="9"/>
+      <c r="D96" s="9"/>
+      <c r="E96" s="9"/>
       <c r="F96" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="5"/>
-      <c r="C97" s="10"/>
-      <c r="D97" s="10"/>
-      <c r="E97" s="10"/>
+      <c r="C97" s="9"/>
+      <c r="D97" s="9"/>
+      <c r="E97" s="9"/>
       <c r="F97" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="5"/>
-      <c r="C98" s="10"/>
-      <c r="D98" s="10"/>
-      <c r="E98" s="10"/>
+      <c r="C98" s="9"/>
+      <c r="D98" s="9"/>
+      <c r="E98" s="9"/>
       <c r="F98" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="5"/>
-      <c r="C99" s="10"/>
-      <c r="D99" s="10"/>
-      <c r="E99" s="10"/>
+      <c r="C99" s="9"/>
+      <c r="D99" s="9"/>
+      <c r="E99" s="9"/>
       <c r="F99" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="5"/>
-      <c r="C100" s="10"/>
-      <c r="D100" s="10"/>
-      <c r="E100" s="10"/>
+      <c r="C100" s="9"/>
+      <c r="D100" s="9"/>
+      <c r="E100" s="9"/>
       <c r="F100" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="5"/>
-      <c r="C101" s="10"/>
-      <c r="D101" s="10"/>
-      <c r="E101" s="10"/>
+      <c r="C101" s="9"/>
+      <c r="D101" s="9"/>
+      <c r="E101" s="9"/>
       <c r="F101" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="5"/>
-      <c r="C102" s="10"/>
-      <c r="D102" s="10"/>
-      <c r="E102" s="10"/>
+      <c r="C102" s="9"/>
+      <c r="D102" s="9"/>
+      <c r="E102" s="9"/>
       <c r="F102" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="5"/>
-      <c r="C103" s="10"/>
-      <c r="D103" s="10"/>
-      <c r="E103" s="10"/>
+      <c r="C103" s="9"/>
+      <c r="D103" s="9"/>
+      <c r="E103" s="9"/>
       <c r="F103" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="5"/>
-      <c r="C104" s="10"/>
-      <c r="D104" s="10"/>
-      <c r="E104" s="10"/>
+      <c r="C104" s="9"/>
+      <c r="D104" s="9"/>
+      <c r="E104" s="9"/>
       <c r="F104" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="5"/>
-      <c r="C105" s="10"/>
-      <c r="D105" s="10"/>
-      <c r="E105" s="10"/>
+      <c r="C105" s="9"/>
+      <c r="D105" s="9"/>
+      <c r="E105" s="9"/>
       <c r="F105" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="5"/>
-      <c r="C106" s="10"/>
-      <c r="D106" s="10"/>
-      <c r="E106" s="10"/>
+      <c r="C106" s="9"/>
+      <c r="D106" s="9"/>
+      <c r="E106" s="9"/>
       <c r="F106" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="5"/>
-      <c r="C107" s="10"/>
-      <c r="D107" s="10"/>
-      <c r="E107" s="10"/>
+      <c r="C107" s="9"/>
+      <c r="D107" s="9"/>
+      <c r="E107" s="9"/>
       <c r="F107" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="5"/>
-      <c r="C108" s="10"/>
-      <c r="D108" s="10"/>
-      <c r="E108" s="10"/>
+      <c r="C108" s="9"/>
+      <c r="D108" s="9"/>
+      <c r="E108" s="9"/>
       <c r="F108" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="5"/>
-      <c r="C109" s="10"/>
-      <c r="D109" s="10"/>
-      <c r="E109" s="10"/>
+      <c r="C109" s="9"/>
+      <c r="D109" s="9"/>
+      <c r="E109" s="9"/>
       <c r="F109" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A110" s="5"/>
+      <c r="C110" s="9"/>
+      <c r="D110" s="9"/>
+      <c r="E110" s="9"/>
+      <c r="F110" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A111" s="5"/>
+      <c r="C111" s="9"/>
+      <c r="D111" s="9"/>
+      <c r="E111" s="9"/>
+      <c r="F111" s="3" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A3:A111">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"Skip"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10:B109" xr:uid="{C4DAE027-D9E5-49CD-83DE-DF6D4AEF99A9}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12:B111" xr:uid="{C4DAE027-D9E5-49CD-83DE-DF6D4AEF99A9}">
       <formula1>ActionTypes</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="C10" r:id="rId1" xr:uid="{AAC55E67-23A3-4AA9-8707-18028DA4614D}"/>
+    <hyperlink ref="C12" r:id="rId1" xr:uid="{AAC55E67-23A3-4AA9-8707-18028DA4614D}"/>
+    <hyperlink ref="F1" r:id="rId2" xr:uid="{9A02F854-77D8-4FBE-A7E3-70A4E48D6A6E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -1764,7 +1808,7 @@
         <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>20</v>
@@ -1783,7 +1827,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3" t="s">
         <v>13</v>
@@ -1811,7 +1855,7 @@
         <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1822,40 +1866,40 @@
         <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" t="s">
         <v>44</v>
       </c>
-      <c r="B7" t="s">
-        <v>45</v>
-      </c>
       <c r="C7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B8" t="s">
         <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B9" t="s">
         <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added support for data records
</commit_message>
<xml_diff>
--- a/src/Mastersign.AutoForm/Template.xlsx
+++ b/src/Mastersign.AutoForm/Template.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Repository\Projekte\OS\Mastersign.AutoForm\src\Mastersign.AutoForm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B6BB73F-AA73-4531-A0A1-6D6B7FA63DF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F17B8AA-3390-4D12-AD1B-F471B175A79A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38130" yWindow="270" windowWidth="23040" windowHeight="18765" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30480" yWindow="810" windowWidth="23040" windowHeight="18765" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Script" sheetId="1" r:id="rId1"/>
-    <sheet name="ActionTypes" sheetId="2" r:id="rId2"/>
+    <sheet name="Records" sheetId="3" r:id="rId2"/>
+    <sheet name="ActionTypes" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="ActionTypeHelp">ActionTypes!$C$2:$C$9</definedName>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="76">
   <si>
     <t>Name</t>
   </si>
@@ -142,9 +143,6 @@
     <t>street</t>
   </si>
   <si>
-    <t>Beispielalee 123a</t>
-  </si>
-  <si>
     <t>city</t>
   </si>
   <si>
@@ -209,6 +207,69 @@
   </si>
   <si>
     <t>https://github.com/mastersign/Mastersign.AutoForm/releases</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Surname</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Street</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Postal Code</t>
+  </si>
+  <si>
+    <t>Mina</t>
+  </si>
+  <si>
+    <t>Musterfrau</t>
+  </si>
+  <si>
+    <t>Musterdorf</t>
+  </si>
+  <si>
+    <t>project</t>
+  </si>
+  <si>
+    <t>Auto Form</t>
+  </si>
+  <si>
+    <t>$(Surname)</t>
+  </si>
+  <si>
+    <t>$(First Name)</t>
+  </si>
+  <si>
+    <t>$(City)</t>
+  </si>
+  <si>
+    <t>$(Postal Code)</t>
+  </si>
+  <si>
+    <t>$(Street) $(Apartment)</t>
+  </si>
+  <si>
+    <t>Apartment</t>
+  </si>
+  <si>
+    <t>44a</t>
+  </si>
+  <si>
+    <t>Musterallee</t>
+  </si>
+  <si>
+    <t>Musterstraße</t>
+  </si>
+  <si>
+    <t>12345</t>
   </si>
 </sst>
 </file>
@@ -312,7 +373,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -325,12 +386,107 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="11">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -617,10 +773,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F111"/>
+  <dimension ref="A1:F112"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -638,7 +794,7 @@
         <v>2</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -667,7 +823,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B7">
         <v>1020</v>
@@ -675,7 +831,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B8">
         <v>1220</v>
@@ -710,7 +866,7 @@
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
       <c r="F11" s="3" t="str">
-        <f t="shared" ref="F11:F21" si="0">IF($B11&lt;&gt;"",_xlfn.XLOOKUP($B11,ActionTypes,ActionTypeParameter) &amp; ": " &amp; _xlfn.XLOOKUP($B11,ActionTypes,ActionTypeHelp),"")</f>
+        <f t="shared" ref="F11:F74" si="0">IF($B11&lt;&gt;"",_xlfn.XLOOKUP($B11,ActionTypes,ActionTypeParameter) &amp; ": " &amp; _xlfn.XLOOKUP($B11,ActionTypes,ActionTypeHelp),"")</f>
         <v/>
       </c>
     </row>
@@ -749,7 +905,7 @@
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>27</v>
@@ -767,7 +923,7 @@
         <v>28</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>29</v>
+        <v>66</v>
       </c>
       <c r="E15" s="9"/>
       <c r="F15" s="3" t="str">
@@ -781,7 +937,7 @@
         <v>30</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>31</v>
+        <v>67</v>
       </c>
       <c r="E16" s="9"/>
       <c r="F16" s="3" t="str">
@@ -795,7 +951,7 @@
         <v>32</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>33</v>
+        <v>70</v>
       </c>
       <c r="E17" s="9"/>
       <c r="F17" s="3" t="str">
@@ -806,10 +962,10 @@
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="C18" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>35</v>
+        <v>68</v>
       </c>
       <c r="E18" s="9"/>
       <c r="F18" s="3" t="str">
@@ -820,10 +976,10 @@
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="C19" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>37</v>
+        <v>69</v>
       </c>
       <c r="E19" s="9"/>
       <c r="F19" s="3" t="str">
@@ -833,59 +989,63 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
-      <c r="B20" t="s">
-        <v>8</v>
-      </c>
       <c r="C20" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="D20" s="10"/>
+        <v>64</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>65</v>
+      </c>
       <c r="E20" s="9"/>
       <c r="F20" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>Label: Interrupt the script execution and wait for the user to proceed.</v>
+        <v/>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
-        <v>52</v>
-      </c>
+      <c r="A21" s="5"/>
       <c r="B21" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="D21" s="9"/>
+        <v>38</v>
+      </c>
+      <c r="D21" s="10"/>
       <c r="E21" s="9"/>
       <c r="F21" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>Selector, [Timeout]: Wait for an element and click on it. Cancel if timeout in milliseconds is reached.</v>
+        <v>Label: Interrupt the script execution and wait for the user to proceed.</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
+      <c r="A22" s="5" t="s">
+        <v>51</v>
+      </c>
       <c r="B22" t="s">
         <v>10</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="D22" s="9"/>
       <c r="E22" s="9"/>
       <c r="F22" s="3" t="str">
-        <f t="shared" ref="F22:F74" si="1">IF($B22&lt;&gt;"",_xlfn.XLOOKUP($B22,ActionTypes,ActionTypeParameter) &amp; ": " &amp; _xlfn.XLOOKUP($B22,ActionTypes,ActionTypeHelp),"")</f>
+        <f t="shared" si="0"/>
         <v>Selector, [Timeout]: Wait for an element and click on it. Cancel if timeout in milliseconds is reached.</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
-      <c r="C23" s="9"/>
+      <c r="B23" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>37</v>
+      </c>
       <c r="D23" s="9"/>
       <c r="E23" s="9"/>
       <c r="F23" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+        <f t="shared" si="0"/>
+        <v>Selector, [Timeout]: Wait for an element and click on it. Cancel if timeout in milliseconds is reached.</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -894,7 +1054,7 @@
       <c r="D24" s="9"/>
       <c r="E24" s="9"/>
       <c r="F24" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -904,7 +1064,7 @@
       <c r="D25" s="9"/>
       <c r="E25" s="9"/>
       <c r="F25" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -914,7 +1074,7 @@
       <c r="D26" s="9"/>
       <c r="E26" s="9"/>
       <c r="F26" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -924,7 +1084,7 @@
       <c r="D27" s="9"/>
       <c r="E27" s="9"/>
       <c r="F27" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -934,7 +1094,7 @@
       <c r="D28" s="9"/>
       <c r="E28" s="9"/>
       <c r="F28" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -944,7 +1104,7 @@
       <c r="D29" s="9"/>
       <c r="E29" s="9"/>
       <c r="F29" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -954,7 +1114,7 @@
       <c r="D30" s="9"/>
       <c r="E30" s="9"/>
       <c r="F30" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -964,7 +1124,7 @@
       <c r="D31" s="9"/>
       <c r="E31" s="9"/>
       <c r="F31" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -974,7 +1134,7 @@
       <c r="D32" s="9"/>
       <c r="E32" s="9"/>
       <c r="F32" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -984,7 +1144,7 @@
       <c r="D33" s="9"/>
       <c r="E33" s="9"/>
       <c r="F33" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -994,7 +1154,7 @@
       <c r="D34" s="9"/>
       <c r="E34" s="9"/>
       <c r="F34" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -1004,7 +1164,7 @@
       <c r="D35" s="9"/>
       <c r="E35" s="9"/>
       <c r="F35" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -1014,7 +1174,7 @@
       <c r="D36" s="9"/>
       <c r="E36" s="9"/>
       <c r="F36" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -1024,7 +1184,7 @@
       <c r="D37" s="9"/>
       <c r="E37" s="9"/>
       <c r="F37" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -1034,7 +1194,7 @@
       <c r="D38" s="9"/>
       <c r="E38" s="9"/>
       <c r="F38" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -1044,7 +1204,7 @@
       <c r="D39" s="9"/>
       <c r="E39" s="9"/>
       <c r="F39" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -1054,7 +1214,7 @@
       <c r="D40" s="9"/>
       <c r="E40" s="9"/>
       <c r="F40" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -1064,7 +1224,7 @@
       <c r="D41" s="9"/>
       <c r="E41" s="9"/>
       <c r="F41" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -1074,7 +1234,7 @@
       <c r="D42" s="9"/>
       <c r="E42" s="9"/>
       <c r="F42" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -1084,7 +1244,7 @@
       <c r="D43" s="9"/>
       <c r="E43" s="9"/>
       <c r="F43" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -1094,7 +1254,7 @@
       <c r="D44" s="9"/>
       <c r="E44" s="9"/>
       <c r="F44" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -1104,7 +1264,7 @@
       <c r="D45" s="9"/>
       <c r="E45" s="9"/>
       <c r="F45" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -1114,7 +1274,7 @@
       <c r="D46" s="9"/>
       <c r="E46" s="9"/>
       <c r="F46" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -1124,7 +1284,7 @@
       <c r="D47" s="9"/>
       <c r="E47" s="9"/>
       <c r="F47" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -1134,7 +1294,7 @@
       <c r="D48" s="9"/>
       <c r="E48" s="9"/>
       <c r="F48" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -1144,7 +1304,7 @@
       <c r="D49" s="9"/>
       <c r="E49" s="9"/>
       <c r="F49" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -1154,7 +1314,7 @@
       <c r="D50" s="9"/>
       <c r="E50" s="9"/>
       <c r="F50" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -1164,7 +1324,7 @@
       <c r="D51" s="9"/>
       <c r="E51" s="9"/>
       <c r="F51" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -1174,7 +1334,7 @@
       <c r="D52" s="9"/>
       <c r="E52" s="9"/>
       <c r="F52" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -1184,7 +1344,7 @@
       <c r="D53" s="9"/>
       <c r="E53" s="9"/>
       <c r="F53" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -1194,7 +1354,7 @@
       <c r="D54" s="9"/>
       <c r="E54" s="9"/>
       <c r="F54" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -1204,7 +1364,7 @@
       <c r="D55" s="9"/>
       <c r="E55" s="9"/>
       <c r="F55" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -1214,7 +1374,7 @@
       <c r="D56" s="9"/>
       <c r="E56" s="9"/>
       <c r="F56" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -1224,7 +1384,7 @@
       <c r="D57" s="9"/>
       <c r="E57" s="9"/>
       <c r="F57" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -1234,7 +1394,7 @@
       <c r="D58" s="9"/>
       <c r="E58" s="9"/>
       <c r="F58" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -1244,7 +1404,7 @@
       <c r="D59" s="9"/>
       <c r="E59" s="9"/>
       <c r="F59" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -1254,7 +1414,7 @@
       <c r="D60" s="9"/>
       <c r="E60" s="9"/>
       <c r="F60" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -1264,7 +1424,7 @@
       <c r="D61" s="9"/>
       <c r="E61" s="9"/>
       <c r="F61" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -1274,7 +1434,7 @@
       <c r="D62" s="9"/>
       <c r="E62" s="9"/>
       <c r="F62" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -1284,7 +1444,7 @@
       <c r="D63" s="9"/>
       <c r="E63" s="9"/>
       <c r="F63" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -1294,7 +1454,7 @@
       <c r="D64" s="9"/>
       <c r="E64" s="9"/>
       <c r="F64" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -1304,7 +1464,7 @@
       <c r="D65" s="9"/>
       <c r="E65" s="9"/>
       <c r="F65" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -1314,7 +1474,7 @@
       <c r="D66" s="9"/>
       <c r="E66" s="9"/>
       <c r="F66" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -1324,7 +1484,7 @@
       <c r="D67" s="9"/>
       <c r="E67" s="9"/>
       <c r="F67" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -1334,7 +1494,7 @@
       <c r="D68" s="9"/>
       <c r="E68" s="9"/>
       <c r="F68" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -1344,7 +1504,7 @@
       <c r="D69" s="9"/>
       <c r="E69" s="9"/>
       <c r="F69" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -1354,7 +1514,7 @@
       <c r="D70" s="9"/>
       <c r="E70" s="9"/>
       <c r="F70" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -1364,7 +1524,7 @@
       <c r="D71" s="9"/>
       <c r="E71" s="9"/>
       <c r="F71" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -1374,7 +1534,7 @@
       <c r="D72" s="9"/>
       <c r="E72" s="9"/>
       <c r="F72" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -1384,7 +1544,7 @@
       <c r="D73" s="9"/>
       <c r="E73" s="9"/>
       <c r="F73" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -1394,7 +1554,7 @@
       <c r="D74" s="9"/>
       <c r="E74" s="9"/>
       <c r="F74" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -1404,7 +1564,7 @@
       <c r="D75" s="9"/>
       <c r="E75" s="9"/>
       <c r="F75" s="3" t="str">
-        <f t="shared" ref="F75:F111" si="2">IF($B75&lt;&gt;"",_xlfn.XLOOKUP($B75,ActionTypes,ActionTypeParameter) &amp; ": " &amp; _xlfn.XLOOKUP($B75,ActionTypes,ActionTypeHelp),"")</f>
+        <f t="shared" ref="F75:F112" si="1">IF($B75&lt;&gt;"",_xlfn.XLOOKUP($B75,ActionTypes,ActionTypeParameter) &amp; ": " &amp; _xlfn.XLOOKUP($B75,ActionTypes,ActionTypeHelp),"")</f>
         <v/>
       </c>
     </row>
@@ -1414,7 +1574,7 @@
       <c r="D76" s="9"/>
       <c r="E76" s="9"/>
       <c r="F76" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -1424,7 +1584,7 @@
       <c r="D77" s="9"/>
       <c r="E77" s="9"/>
       <c r="F77" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -1434,7 +1594,7 @@
       <c r="D78" s="9"/>
       <c r="E78" s="9"/>
       <c r="F78" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -1444,7 +1604,7 @@
       <c r="D79" s="9"/>
       <c r="E79" s="9"/>
       <c r="F79" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -1454,7 +1614,7 @@
       <c r="D80" s="9"/>
       <c r="E80" s="9"/>
       <c r="F80" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -1464,7 +1624,7 @@
       <c r="D81" s="9"/>
       <c r="E81" s="9"/>
       <c r="F81" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -1474,7 +1634,7 @@
       <c r="D82" s="9"/>
       <c r="E82" s="9"/>
       <c r="F82" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -1484,7 +1644,7 @@
       <c r="D83" s="9"/>
       <c r="E83" s="9"/>
       <c r="F83" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -1494,7 +1654,7 @@
       <c r="D84" s="9"/>
       <c r="E84" s="9"/>
       <c r="F84" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -1504,7 +1664,7 @@
       <c r="D85" s="9"/>
       <c r="E85" s="9"/>
       <c r="F85" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -1514,7 +1674,7 @@
       <c r="D86" s="9"/>
       <c r="E86" s="9"/>
       <c r="F86" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -1524,7 +1684,7 @@
       <c r="D87" s="9"/>
       <c r="E87" s="9"/>
       <c r="F87" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -1534,7 +1694,7 @@
       <c r="D88" s="9"/>
       <c r="E88" s="9"/>
       <c r="F88" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -1544,7 +1704,7 @@
       <c r="D89" s="9"/>
       <c r="E89" s="9"/>
       <c r="F89" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -1554,7 +1714,7 @@
       <c r="D90" s="9"/>
       <c r="E90" s="9"/>
       <c r="F90" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -1564,7 +1724,7 @@
       <c r="D91" s="9"/>
       <c r="E91" s="9"/>
       <c r="F91" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -1574,7 +1734,7 @@
       <c r="D92" s="9"/>
       <c r="E92" s="9"/>
       <c r="F92" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -1584,7 +1744,7 @@
       <c r="D93" s="9"/>
       <c r="E93" s="9"/>
       <c r="F93" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -1594,7 +1754,7 @@
       <c r="D94" s="9"/>
       <c r="E94" s="9"/>
       <c r="F94" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -1604,7 +1764,7 @@
       <c r="D95" s="9"/>
       <c r="E95" s="9"/>
       <c r="F95" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -1614,7 +1774,7 @@
       <c r="D96" s="9"/>
       <c r="E96" s="9"/>
       <c r="F96" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -1624,7 +1784,7 @@
       <c r="D97" s="9"/>
       <c r="E97" s="9"/>
       <c r="F97" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -1634,7 +1794,7 @@
       <c r="D98" s="9"/>
       <c r="E98" s="9"/>
       <c r="F98" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -1644,7 +1804,7 @@
       <c r="D99" s="9"/>
       <c r="E99" s="9"/>
       <c r="F99" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -1654,7 +1814,7 @@
       <c r="D100" s="9"/>
       <c r="E100" s="9"/>
       <c r="F100" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -1664,7 +1824,7 @@
       <c r="D101" s="9"/>
       <c r="E101" s="9"/>
       <c r="F101" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -1674,7 +1834,7 @@
       <c r="D102" s="9"/>
       <c r="E102" s="9"/>
       <c r="F102" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -1684,7 +1844,7 @@
       <c r="D103" s="9"/>
       <c r="E103" s="9"/>
       <c r="F103" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -1694,7 +1854,7 @@
       <c r="D104" s="9"/>
       <c r="E104" s="9"/>
       <c r="F104" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -1704,7 +1864,7 @@
       <c r="D105" s="9"/>
       <c r="E105" s="9"/>
       <c r="F105" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -1714,7 +1874,7 @@
       <c r="D106" s="9"/>
       <c r="E106" s="9"/>
       <c r="F106" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -1724,7 +1884,7 @@
       <c r="D107" s="9"/>
       <c r="E107" s="9"/>
       <c r="F107" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -1734,7 +1894,7 @@
       <c r="D108" s="9"/>
       <c r="E108" s="9"/>
       <c r="F108" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -1744,7 +1904,7 @@
       <c r="D109" s="9"/>
       <c r="E109" s="9"/>
       <c r="F109" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -1754,7 +1914,7 @@
       <c r="D110" s="9"/>
       <c r="E110" s="9"/>
       <c r="F110" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -1764,18 +1924,38 @@
       <c r="D111" s="9"/>
       <c r="E111" s="9"/>
       <c r="F111" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A112" s="5"/>
+      <c r="C112" s="9"/>
+      <c r="D112" s="9"/>
+      <c r="E112" s="9"/>
+      <c r="F112" s="3" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A3:A111">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+  <conditionalFormatting sqref="A3:A112">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
       <formula>"Skip"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B11:B112">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+      <formula>"Pause"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C11:E112">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="$(">
+      <formula>NOT(ISERROR(SEARCH("$(",C11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12:B111" xr:uid="{C4DAE027-D9E5-49CD-83DE-DF6D4AEF99A9}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12:B112" xr:uid="{C4DAE027-D9E5-49CD-83DE-DF6D4AEF99A9}">
       <formula1>ActionTypes</formula1>
     </dataValidation>
   </dataValidations>
@@ -1789,6 +1969,96 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{067C52CF-AB48-4CA8-AE44-EF0C4C1AFEE5}">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>101</v>
+      </c>
+      <c r="B2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E2">
+        <v>123</v>
+      </c>
+      <c r="F2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>102</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E7937D3-1BD0-4B7A-9ECB-0067EE47F0B1}">
   <dimension ref="A1:C9"/>
   <sheetViews>
@@ -1804,13 +2074,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1827,7 +2097,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B3" t="s">
         <v>13</v>
@@ -1855,7 +2125,7 @@
         <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1866,40 +2136,40 @@
         <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" t="s">
         <v>43</v>
       </c>
-      <c r="B7" t="s">
-        <v>44</v>
-      </c>
       <c r="C7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B8" t="s">
         <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B9" t="s">
         <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implemented support for conditional actions
</commit_message>
<xml_diff>
--- a/src/Mastersign.AutoForm/Template.xlsx
+++ b/src/Mastersign.AutoForm/Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Repository\Projekte\OS\Mastersign.AutoForm\src\Mastersign.AutoForm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F17B8AA-3390-4D12-AD1B-F471B175A79A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F926E6E1-757B-46E3-91C5-2D30B567177A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30480" yWindow="810" windowWidth="23040" windowHeight="18765" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Script" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="78">
   <si>
     <t>Name</t>
   </si>
@@ -260,16 +260,22 @@
     <t>Apartment</t>
   </si>
   <si>
-    <t>44a</t>
-  </si>
-  <si>
-    <t>Musterallee</t>
-  </si>
-  <si>
     <t>Musterstraße</t>
   </si>
   <si>
     <t>12345</t>
+  </si>
+  <si>
+    <t>Condition</t>
+  </si>
+  <si>
+    <t>$(Street)</t>
+  </si>
+  <si>
+    <t>Auto-Help</t>
+  </si>
+  <si>
+    <t>Section</t>
   </si>
 </sst>
 </file>
@@ -392,31 +398,18 @@
     <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="5">
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -434,56 +427,6 @@
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -773,7 +716,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F112"/>
+  <dimension ref="A1:G112"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
@@ -785,23 +728,25 @@
     <col min="2" max="2" width="12.140625" customWidth="1"/>
     <col min="3" max="3" width="48.85546875" customWidth="1"/>
     <col min="4" max="4" width="14.42578125" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" customWidth="1"/>
-    <col min="6" max="6" width="108.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13.7109375" customWidth="1"/>
+    <col min="7" max="7" width="108.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="5" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" s="5" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="G1" s="11" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>0</v>
       </c>
@@ -809,7 +754,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>1</v>
       </c>
@@ -817,11 +762,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>52</v>
       </c>
@@ -829,7 +774,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>53</v>
       </c>
@@ -837,10 +782,10 @@
         <v>1220</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="4" t="s">
         <v>21</v>
@@ -855,22 +800,26 @@
         <v>24</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
-      <c r="F11" s="3" t="str">
-        <f t="shared" ref="F11:F74" si="0">IF($B11&lt;&gt;"",_xlfn.XLOOKUP($B11,ActionTypes,ActionTypeParameter) &amp; ": " &amp; _xlfn.XLOOKUP($B11,ActionTypes,ActionTypeHelp),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F11" s="9"/>
+      <c r="G11" s="3" t="str">
+        <f t="shared" ref="G11:G74" si="0">IF($B11&lt;&gt;"",_xlfn.XLOOKUP($B11,ActionTypes,ActionTypeParameter) &amp; ": " &amp; _xlfn.XLOOKUP($B11,ActionTypes,ActionTypeHelp),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" t="s">
         <v>6</v>
@@ -880,12 +829,13 @@
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
-      <c r="F12" s="3" t="str">
+      <c r="F12" s="9"/>
+      <c r="G12" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Url, [Timeout]: Navigate to the given URL. Cancel if timeout in milliseconds is reached.</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" t="s">
         <v>9</v>
@@ -897,12 +847,13 @@
         <v>500</v>
       </c>
       <c r="E13" s="9"/>
-      <c r="F13" s="3" t="str">
+      <c r="F13" s="9"/>
+      <c r="G13" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Selector, [Timeout]: Wait for an element to be present and visible/hidden. Cancel if timeout in milliseconds is reached.</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" t="s">
         <v>40</v>
@@ -912,12 +863,13 @@
       </c>
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
-      <c r="F14" s="3" t="str">
+      <c r="F14" s="9"/>
+      <c r="G14" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Selector, [Timeout], …Fields: Wait for a form and fill its fields. Cancel if timeout in milliseconds is reached.</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="C15" s="9" t="s">
         <v>28</v>
@@ -926,12 +878,13 @@
         <v>66</v>
       </c>
       <c r="E15" s="9"/>
-      <c r="F15" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F15" s="9"/>
+      <c r="G15" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="C16" s="9" t="s">
         <v>30</v>
@@ -940,12 +893,13 @@
         <v>67</v>
       </c>
       <c r="E16" s="9"/>
-      <c r="F16" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F16" s="9"/>
+      <c r="G16" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="C17" s="9" t="s">
         <v>32</v>
@@ -954,12 +908,15 @@
         <v>70</v>
       </c>
       <c r="E17" s="9"/>
-      <c r="F17" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F17" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="G17" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="C18" s="9" t="s">
         <v>33</v>
@@ -968,12 +925,13 @@
         <v>68</v>
       </c>
       <c r="E18" s="9"/>
-      <c r="F18" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F18" s="9"/>
+      <c r="G18" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="C19" s="9" t="s">
         <v>35</v>
@@ -982,12 +940,13 @@
         <v>69</v>
       </c>
       <c r="E19" s="9"/>
-      <c r="F19" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F19" s="9"/>
+      <c r="G19" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="C20" s="9" t="s">
         <v>64</v>
@@ -996,12 +955,13 @@
         <v>65</v>
       </c>
       <c r="E20" s="9"/>
-      <c r="F20" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F20" s="9"/>
+      <c r="G20" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="B21" t="s">
         <v>8</v>
@@ -1011,12 +971,13 @@
       </c>
       <c r="D21" s="10"/>
       <c r="E21" s="9"/>
-      <c r="F21" s="3" t="str">
+      <c r="F21" s="9"/>
+      <c r="G21" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Label: Interrupt the script execution and wait for the user to proceed.</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>51</v>
       </c>
@@ -1028,12 +989,13 @@
       </c>
       <c r="D22" s="9"/>
       <c r="E22" s="9"/>
-      <c r="F22" s="3" t="str">
+      <c r="F22" s="9"/>
+      <c r="G22" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Selector, [Timeout]: Wait for an element and click on it. Cancel if timeout in milliseconds is reached.</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="B23" t="s">
         <v>10</v>
@@ -1043,915 +1005,1013 @@
       </c>
       <c r="D23" s="9"/>
       <c r="E23" s="9"/>
-      <c r="F23" s="3" t="str">
+      <c r="F23" s="9"/>
+      <c r="G23" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Selector, [Timeout]: Wait for an element and click on it. Cancel if timeout in milliseconds is reached.</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
       <c r="E24" s="9"/>
-      <c r="F24" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F24" s="9"/>
+      <c r="G24" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
       <c r="E25" s="9"/>
-      <c r="F25" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F25" s="9"/>
+      <c r="G25" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="C26" s="9"/>
       <c r="D26" s="9"/>
       <c r="E26" s="9"/>
-      <c r="F26" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F26" s="9"/>
+      <c r="G26" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
       <c r="E27" s="9"/>
-      <c r="F27" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F27" s="9"/>
+      <c r="G27" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
       <c r="C28" s="9"/>
       <c r="D28" s="9"/>
       <c r="E28" s="9"/>
-      <c r="F28" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F28" s="9"/>
+      <c r="G28" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
       <c r="C29" s="9"/>
       <c r="D29" s="9"/>
       <c r="E29" s="9"/>
-      <c r="F29" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F29" s="9"/>
+      <c r="G29" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
       <c r="C30" s="9"/>
       <c r="D30" s="9"/>
       <c r="E30" s="9"/>
-      <c r="F30" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F30" s="9"/>
+      <c r="G30" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
       <c r="C31" s="9"/>
       <c r="D31" s="9"/>
       <c r="E31" s="9"/>
-      <c r="F31" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F31" s="9"/>
+      <c r="G31" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
       <c r="C32" s="9"/>
       <c r="D32" s="9"/>
       <c r="E32" s="9"/>
-      <c r="F32" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F32" s="9"/>
+      <c r="G32" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
       <c r="C33" s="9"/>
       <c r="D33" s="9"/>
       <c r="E33" s="9"/>
-      <c r="F33" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F33" s="9"/>
+      <c r="G33" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="5"/>
       <c r="C34" s="9"/>
       <c r="D34" s="9"/>
       <c r="E34" s="9"/>
-      <c r="F34" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F34" s="9"/>
+      <c r="G34" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="5"/>
       <c r="C35" s="9"/>
       <c r="D35" s="9"/>
       <c r="E35" s="9"/>
-      <c r="F35" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F35" s="9"/>
+      <c r="G35" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="5"/>
       <c r="C36" s="9"/>
       <c r="D36" s="9"/>
       <c r="E36" s="9"/>
-      <c r="F36" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F36" s="9"/>
+      <c r="G36" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="5"/>
       <c r="C37" s="9"/>
       <c r="D37" s="9"/>
       <c r="E37" s="9"/>
-      <c r="F37" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F37" s="9"/>
+      <c r="G37" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="5"/>
       <c r="C38" s="9"/>
       <c r="D38" s="9"/>
       <c r="E38" s="9"/>
-      <c r="F38" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F38" s="9"/>
+      <c r="G38" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="5"/>
       <c r="C39" s="9"/>
       <c r="D39" s="9"/>
       <c r="E39" s="9"/>
-      <c r="F39" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F39" s="9"/>
+      <c r="G39" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="5"/>
       <c r="C40" s="9"/>
       <c r="D40" s="9"/>
       <c r="E40" s="9"/>
-      <c r="F40" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F40" s="9"/>
+      <c r="G40" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="5"/>
       <c r="C41" s="9"/>
       <c r="D41" s="9"/>
       <c r="E41" s="9"/>
-      <c r="F41" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F41" s="9"/>
+      <c r="G41" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="5"/>
       <c r="C42" s="9"/>
       <c r="D42" s="9"/>
       <c r="E42" s="9"/>
-      <c r="F42" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F42" s="9"/>
+      <c r="G42" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="5"/>
       <c r="C43" s="9"/>
       <c r="D43" s="9"/>
       <c r="E43" s="9"/>
-      <c r="F43" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F43" s="9"/>
+      <c r="G43" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="5"/>
       <c r="C44" s="9"/>
       <c r="D44" s="9"/>
       <c r="E44" s="9"/>
-      <c r="F44" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F44" s="9"/>
+      <c r="G44" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="5"/>
       <c r="C45" s="9"/>
       <c r="D45" s="9"/>
       <c r="E45" s="9"/>
-      <c r="F45" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F45" s="9"/>
+      <c r="G45" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="5"/>
       <c r="C46" s="9"/>
       <c r="D46" s="9"/>
       <c r="E46" s="9"/>
-      <c r="F46" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F46" s="9"/>
+      <c r="G46" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="5"/>
       <c r="C47" s="9"/>
       <c r="D47" s="9"/>
       <c r="E47" s="9"/>
-      <c r="F47" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F47" s="9"/>
+      <c r="G47" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="5"/>
       <c r="C48" s="9"/>
       <c r="D48" s="9"/>
       <c r="E48" s="9"/>
-      <c r="F48" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F48" s="9"/>
+      <c r="G48" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="5"/>
       <c r="C49" s="9"/>
       <c r="D49" s="9"/>
       <c r="E49" s="9"/>
-      <c r="F49" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F49" s="9"/>
+      <c r="G49" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="5"/>
       <c r="C50" s="9"/>
       <c r="D50" s="9"/>
       <c r="E50" s="9"/>
-      <c r="F50" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F50" s="9"/>
+      <c r="G50" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="5"/>
       <c r="C51" s="9"/>
       <c r="D51" s="9"/>
       <c r="E51" s="9"/>
-      <c r="F51" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F51" s="9"/>
+      <c r="G51" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="5"/>
       <c r="C52" s="9"/>
       <c r="D52" s="9"/>
       <c r="E52" s="9"/>
-      <c r="F52" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F52" s="9"/>
+      <c r="G52" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="5"/>
       <c r="C53" s="9"/>
       <c r="D53" s="9"/>
       <c r="E53" s="9"/>
-      <c r="F53" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F53" s="9"/>
+      <c r="G53" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="5"/>
       <c r="C54" s="9"/>
       <c r="D54" s="9"/>
       <c r="E54" s="9"/>
-      <c r="F54" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F54" s="9"/>
+      <c r="G54" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="5"/>
       <c r="C55" s="9"/>
       <c r="D55" s="9"/>
       <c r="E55" s="9"/>
-      <c r="F55" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F55" s="9"/>
+      <c r="G55" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="5"/>
       <c r="C56" s="9"/>
       <c r="D56" s="9"/>
       <c r="E56" s="9"/>
-      <c r="F56" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F56" s="9"/>
+      <c r="G56" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="5"/>
       <c r="C57" s="9"/>
       <c r="D57" s="9"/>
       <c r="E57" s="9"/>
-      <c r="F57" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F57" s="9"/>
+      <c r="G57" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="5"/>
       <c r="C58" s="9"/>
       <c r="D58" s="9"/>
       <c r="E58" s="9"/>
-      <c r="F58" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F58" s="9"/>
+      <c r="G58" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="5"/>
       <c r="C59" s="9"/>
       <c r="D59" s="9"/>
       <c r="E59" s="9"/>
-      <c r="F59" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F59" s="9"/>
+      <c r="G59" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="5"/>
       <c r="C60" s="9"/>
       <c r="D60" s="9"/>
       <c r="E60" s="9"/>
-      <c r="F60" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F60" s="9"/>
+      <c r="G60" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="5"/>
       <c r="C61" s="9"/>
       <c r="D61" s="9"/>
       <c r="E61" s="9"/>
-      <c r="F61" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F61" s="9"/>
+      <c r="G61" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="5"/>
       <c r="C62" s="9"/>
       <c r="D62" s="9"/>
       <c r="E62" s="9"/>
-      <c r="F62" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F62" s="9"/>
+      <c r="G62" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="5"/>
       <c r="C63" s="9"/>
       <c r="D63" s="9"/>
       <c r="E63" s="9"/>
-      <c r="F63" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F63" s="9"/>
+      <c r="G63" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="5"/>
       <c r="C64" s="9"/>
       <c r="D64" s="9"/>
       <c r="E64" s="9"/>
-      <c r="F64" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F64" s="9"/>
+      <c r="G64" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="5"/>
       <c r="C65" s="9"/>
       <c r="D65" s="9"/>
       <c r="E65" s="9"/>
-      <c r="F65" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F65" s="9"/>
+      <c r="G65" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="5"/>
       <c r="C66" s="9"/>
       <c r="D66" s="9"/>
       <c r="E66" s="9"/>
-      <c r="F66" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F66" s="9"/>
+      <c r="G66" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="5"/>
       <c r="C67" s="9"/>
       <c r="D67" s="9"/>
       <c r="E67" s="9"/>
-      <c r="F67" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F67" s="9"/>
+      <c r="G67" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="5"/>
       <c r="C68" s="9"/>
       <c r="D68" s="9"/>
       <c r="E68" s="9"/>
-      <c r="F68" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F68" s="9"/>
+      <c r="G68" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="5"/>
       <c r="C69" s="9"/>
       <c r="D69" s="9"/>
       <c r="E69" s="9"/>
-      <c r="F69" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F69" s="9"/>
+      <c r="G69" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="5"/>
       <c r="C70" s="9"/>
       <c r="D70" s="9"/>
       <c r="E70" s="9"/>
-      <c r="F70" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F70" s="9"/>
+      <c r="G70" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="5"/>
       <c r="C71" s="9"/>
       <c r="D71" s="9"/>
       <c r="E71" s="9"/>
-      <c r="F71" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F71" s="9"/>
+      <c r="G71" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="5"/>
       <c r="C72" s="9"/>
       <c r="D72" s="9"/>
       <c r="E72" s="9"/>
-      <c r="F72" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F72" s="9"/>
+      <c r="G72" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="5"/>
       <c r="C73" s="9"/>
       <c r="D73" s="9"/>
       <c r="E73" s="9"/>
-      <c r="F73" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F73" s="9"/>
+      <c r="G73" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="5"/>
       <c r="C74" s="9"/>
       <c r="D74" s="9"/>
       <c r="E74" s="9"/>
-      <c r="F74" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F74" s="9"/>
+      <c r="G74" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="5"/>
       <c r="C75" s="9"/>
       <c r="D75" s="9"/>
       <c r="E75" s="9"/>
-      <c r="F75" s="3" t="str">
-        <f t="shared" ref="F75:F112" si="1">IF($B75&lt;&gt;"",_xlfn.XLOOKUP($B75,ActionTypes,ActionTypeParameter) &amp; ": " &amp; _xlfn.XLOOKUP($B75,ActionTypes,ActionTypeHelp),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F75" s="9"/>
+      <c r="G75" s="3" t="str">
+        <f t="shared" ref="G75:G112" si="1">IF($B75&lt;&gt;"",_xlfn.XLOOKUP($B75,ActionTypes,ActionTypeParameter) &amp; ": " &amp; _xlfn.XLOOKUP($B75,ActionTypes,ActionTypeHelp),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="5"/>
       <c r="C76" s="9"/>
       <c r="D76" s="9"/>
       <c r="E76" s="9"/>
-      <c r="F76" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F76" s="9"/>
+      <c r="G76" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="5"/>
       <c r="C77" s="9"/>
       <c r="D77" s="9"/>
       <c r="E77" s="9"/>
-      <c r="F77" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F77" s="9"/>
+      <c r="G77" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="5"/>
       <c r="C78" s="9"/>
       <c r="D78" s="9"/>
       <c r="E78" s="9"/>
-      <c r="F78" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F78" s="9"/>
+      <c r="G78" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="5"/>
       <c r="C79" s="9"/>
       <c r="D79" s="9"/>
       <c r="E79" s="9"/>
-      <c r="F79" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F79" s="9"/>
+      <c r="G79" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="5"/>
       <c r="C80" s="9"/>
       <c r="D80" s="9"/>
       <c r="E80" s="9"/>
-      <c r="F80" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F80" s="9"/>
+      <c r="G80" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="5"/>
       <c r="C81" s="9"/>
       <c r="D81" s="9"/>
       <c r="E81" s="9"/>
-      <c r="F81" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F81" s="9"/>
+      <c r="G81" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="5"/>
       <c r="C82" s="9"/>
       <c r="D82" s="9"/>
       <c r="E82" s="9"/>
-      <c r="F82" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F82" s="9"/>
+      <c r="G82" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="5"/>
       <c r="C83" s="9"/>
       <c r="D83" s="9"/>
       <c r="E83" s="9"/>
-      <c r="F83" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F83" s="9"/>
+      <c r="G83" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="5"/>
       <c r="C84" s="9"/>
       <c r="D84" s="9"/>
       <c r="E84" s="9"/>
-      <c r="F84" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F84" s="9"/>
+      <c r="G84" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="5"/>
       <c r="C85" s="9"/>
       <c r="D85" s="9"/>
       <c r="E85" s="9"/>
-      <c r="F85" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F85" s="9"/>
+      <c r="G85" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="5"/>
       <c r="C86" s="9"/>
       <c r="D86" s="9"/>
       <c r="E86" s="9"/>
-      <c r="F86" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F86" s="9"/>
+      <c r="G86" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="5"/>
       <c r="C87" s="9"/>
       <c r="D87" s="9"/>
       <c r="E87" s="9"/>
-      <c r="F87" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F87" s="9"/>
+      <c r="G87" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="5"/>
       <c r="C88" s="9"/>
       <c r="D88" s="9"/>
       <c r="E88" s="9"/>
-      <c r="F88" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F88" s="9"/>
+      <c r="G88" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="5"/>
       <c r="C89" s="9"/>
       <c r="D89" s="9"/>
       <c r="E89" s="9"/>
-      <c r="F89" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F89" s="9"/>
+      <c r="G89" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="5"/>
       <c r="C90" s="9"/>
       <c r="D90" s="9"/>
       <c r="E90" s="9"/>
-      <c r="F90" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F90" s="9"/>
+      <c r="G90" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="5"/>
       <c r="C91" s="9"/>
       <c r="D91" s="9"/>
       <c r="E91" s="9"/>
-      <c r="F91" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F91" s="9"/>
+      <c r="G91" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="5"/>
       <c r="C92" s="9"/>
       <c r="D92" s="9"/>
       <c r="E92" s="9"/>
-      <c r="F92" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F92" s="9"/>
+      <c r="G92" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="5"/>
       <c r="C93" s="9"/>
       <c r="D93" s="9"/>
       <c r="E93" s="9"/>
-      <c r="F93" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F93" s="9"/>
+      <c r="G93" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="5"/>
       <c r="C94" s="9"/>
       <c r="D94" s="9"/>
       <c r="E94" s="9"/>
-      <c r="F94" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F94" s="9"/>
+      <c r="G94" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="5"/>
       <c r="C95" s="9"/>
       <c r="D95" s="9"/>
       <c r="E95" s="9"/>
-      <c r="F95" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F95" s="9"/>
+      <c r="G95" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="5"/>
       <c r="C96" s="9"/>
       <c r="D96" s="9"/>
       <c r="E96" s="9"/>
-      <c r="F96" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F96" s="9"/>
+      <c r="G96" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="5"/>
       <c r="C97" s="9"/>
       <c r="D97" s="9"/>
       <c r="E97" s="9"/>
-      <c r="F97" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F97" s="9"/>
+      <c r="G97" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="5"/>
       <c r="C98" s="9"/>
       <c r="D98" s="9"/>
       <c r="E98" s="9"/>
-      <c r="F98" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F98" s="9"/>
+      <c r="G98" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="5"/>
       <c r="C99" s="9"/>
       <c r="D99" s="9"/>
       <c r="E99" s="9"/>
-      <c r="F99" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F99" s="9"/>
+      <c r="G99" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="5"/>
       <c r="C100" s="9"/>
       <c r="D100" s="9"/>
       <c r="E100" s="9"/>
-      <c r="F100" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F100" s="9"/>
+      <c r="G100" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="5"/>
       <c r="C101" s="9"/>
       <c r="D101" s="9"/>
       <c r="E101" s="9"/>
-      <c r="F101" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F101" s="9"/>
+      <c r="G101" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="5"/>
       <c r="C102" s="9"/>
       <c r="D102" s="9"/>
       <c r="E102" s="9"/>
-      <c r="F102" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F102" s="9"/>
+      <c r="G102" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="5"/>
       <c r="C103" s="9"/>
       <c r="D103" s="9"/>
       <c r="E103" s="9"/>
-      <c r="F103" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F103" s="9"/>
+      <c r="G103" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="5"/>
       <c r="C104" s="9"/>
       <c r="D104" s="9"/>
       <c r="E104" s="9"/>
-      <c r="F104" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F104" s="9"/>
+      <c r="G104" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="5"/>
       <c r="C105" s="9"/>
       <c r="D105" s="9"/>
       <c r="E105" s="9"/>
-      <c r="F105" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F105" s="9"/>
+      <c r="G105" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="5"/>
       <c r="C106" s="9"/>
       <c r="D106" s="9"/>
       <c r="E106" s="9"/>
-      <c r="F106" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F106" s="9"/>
+      <c r="G106" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="5"/>
       <c r="C107" s="9"/>
       <c r="D107" s="9"/>
       <c r="E107" s="9"/>
-      <c r="F107" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F107" s="9"/>
+      <c r="G107" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="5"/>
       <c r="C108" s="9"/>
       <c r="D108" s="9"/>
       <c r="E108" s="9"/>
-      <c r="F108" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F108" s="9"/>
+      <c r="G108" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="5"/>
       <c r="C109" s="9"/>
       <c r="D109" s="9"/>
       <c r="E109" s="9"/>
-      <c r="F109" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F109" s="9"/>
+      <c r="G109" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="5"/>
       <c r="C110" s="9"/>
       <c r="D110" s="9"/>
       <c r="E110" s="9"/>
-      <c r="F110" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F110" s="9"/>
+      <c r="G110" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="5"/>
       <c r="C111" s="9"/>
       <c r="D111" s="9"/>
       <c r="E111" s="9"/>
-      <c r="F111" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F111" s="9"/>
+      <c r="G111" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="5"/>
       <c r="C112" s="9"/>
       <c r="D112" s="9"/>
       <c r="E112" s="9"/>
-      <c r="F112" s="3" t="str">
+      <c r="F112" s="9"/>
+      <c r="G112" s="3" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:A112">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"Skip"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11:B112">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"Pause"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11:E112">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="$(">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="$(">
       <formula>NOT(ISERROR(SEARCH("$(",C11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F11:F112">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="2">
+      <formula>LEN(TRIM(F11))&gt;0</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="$(">
+      <formula>NOT(ISERROR(SEARCH("$(",F11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -1961,7 +2021,7 @@
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="C12" r:id="rId1" xr:uid="{AAC55E67-23A3-4AA9-8707-18028DA4614D}"/>
-    <hyperlink ref="F1" r:id="rId2" xr:uid="{9A02F854-77D8-4FBE-A7E3-70A4E48D6A6E}"/>
+    <hyperlink ref="G1" r:id="rId2" xr:uid="{9A02F854-77D8-4FBE-A7E3-70A4E48D6A6E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
@@ -2018,7 +2078,7 @@
         <v>62</v>
       </c>
       <c r="D2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E2">
         <v>123</v>
@@ -2040,17 +2100,11 @@
       <c r="C3" t="s">
         <v>29</v>
       </c>
-      <c r="D3" t="s">
-        <v>73</v>
-      </c>
-      <c r="E3" t="s">
-        <v>72</v>
-      </c>
       <c r="F3" t="s">
         <v>63</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
minor improvements and fixes
</commit_message>
<xml_diff>
--- a/src/Mastersign.AutoForm/Template.xlsx
+++ b/src/Mastersign.AutoForm/Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repo\projects\OS\Mastersign.AutoForm\src\Mastersign.AutoForm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68F46191-C126-4EF9-BC4F-5A70ED5AADDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE189E5A-F2AA-45AE-9C2D-68093F5F3D2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3900" yWindow="615" windowWidth="15570" windowHeight="20985" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Script" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="86">
   <si>
     <t>Name</t>
   </si>
@@ -297,6 +297,9 @@
   </si>
   <si>
     <t>Reload the current page. Cancel if timeout in milliseconds is reached.</t>
+  </si>
+  <si>
+    <t>Selector, Visible, [Timeout]</t>
   </si>
 </sst>
 </file>
@@ -763,7 +766,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G114"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
@@ -903,7 +906,7 @@
       <c r="F14" s="9"/>
       <c r="G14" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>Selector, [Timeout]: Wait for an element to be present and visible/hidden. Cancel if timeout in milliseconds is reached.</v>
+        <v>Selector, Visible, [Timeout]: Wait for an element to be present and visible/hidden. Cancel if timeout in milliseconds is reached.</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -2192,7 +2195,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E7937D3-1BD0-4B7A-9ECB-0067EE47F0B1}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
@@ -2263,7 +2266,7 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>85</v>
       </c>
       <c r="C6" t="s">
         <v>45</v>

</xml_diff>